<commit_message>
changed from monthly to weekly
</commit_message>
<xml_diff>
--- a/df_final.xlsx
+++ b/df_final.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -56,19 +56,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44408</v>
+        <v>44381</v>
       </c>
       <c r="C2" t="n">
-        <v>1040.323457256861</v>
+        <v>540.2418001318053</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -502,7 +502,259 @@
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44388</v>
+      </c>
+      <c r="C3" t="n">
+        <v>632.3650882947178</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44395</v>
+      </c>
+      <c r="C4" t="n">
+        <v>783.053048224588</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44402</v>
+      </c>
+      <c r="C5" t="n">
+        <v>942.5301754650492</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44409</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1051.262986828038</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1083.344825274121</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1051.343280169708</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C9" t="n">
+        <v>975.2416540263248</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44437</v>
+      </c>
+      <c r="C10" t="n">
+        <v>859.0627157860984</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44444</v>
+      </c>
+      <c r="C11" t="n">
+        <v>704.1046460870393</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VETINA-Antibiotics -Cat_2</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2021-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>44381</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>